<commit_message>
Forms synchronized with database
</commit_message>
<xml_diff>
--- a/Database/mandatory_fields.xlsx
+++ b/Database/mandatory_fields.xlsx
@@ -23,15 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
-    <t>Help_Request</t>
-  </si>
-  <si>
-    <t>Information</t>
-  </si>
-  <si>
-    <t>Provide_Help</t>
-  </si>
-  <si>
     <t>message_id</t>
   </si>
   <si>
@@ -63,6 +54,15 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Offer support</t>
+  </si>
+  <si>
+    <t>Need support and emergency</t>
   </si>
 </sst>
 </file>
@@ -444,129 +444,130 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="4" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>

</xml_diff>

<commit_message>
Fix of Right-click-menu position Update of mandatory fields of specific Databaseattributes
</commit_message>
<xml_diff>
--- a/Database/mandatory_fields.xlsx
+++ b/Database/mandatory_fields.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\Disaster-Management-2014\Database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="19260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>message_id</t>
   </si>
@@ -44,9 +44,6 @@
     <t>date_of_creation</t>
   </si>
   <si>
-    <t>date of creation</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -56,13 +53,13 @@
     <t>title</t>
   </si>
   <si>
-    <t>Message</t>
-  </si>
-  <si>
     <t>Offer support</t>
   </si>
   <si>
     <t>Need support and emergency</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -102,29 +99,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -197,7 +194,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,7 +229,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,29 +440,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="4" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -487,18 +484,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -509,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -520,18 +517,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -542,48 +539,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -593,9 +594,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -605,8 +611,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated database schema to current used one
- Added SRID_ID information
- Added hulluser_id
- Removed unused information
</commit_message>
<xml_diff>
--- a/Database/mandatory_fields.xlsx
+++ b/Database/mandatory_fields.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schlomm\Documents\GitHub\Disaster-Management-2014\Database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="19260"/>
   </bookViews>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t>message_id</t>
   </si>
@@ -33,9 +38,6 @@
   </si>
   <si>
     <t>time_start</t>
-  </si>
-  <si>
-    <t>time_stop</t>
   </si>
   <si>
     <t>description</t>
@@ -438,31 +440,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="4" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -473,7 +475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -484,18 +486,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -506,40 +508,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -548,35 +548,26 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -594,7 +585,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -611,7 +602,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>